<commit_message>
Signed-off-by: Sheldon Henrique <tifmepo@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/corona.xlsx
+++ b/corona.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-Gamer\Desktop\corona\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C7385D-71B6-4344-A0D2-FE174ED4CB92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7017581C-F455-40C2-8F47-FB5ED98B4714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30410" yWindow="2490" windowWidth="38620" windowHeight="21000" xr2:uid="{4C98B353-EDBB-48FF-AC02-0102F8101F02}"/>
+    <workbookView xWindow="-2140" yWindow="1090" windowWidth="38620" windowHeight="21000" xr2:uid="{4C98B353-EDBB-48FF-AC02-0102F8101F02}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -92,11 +92,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,7 +415,7 @@
   <dimension ref="A1:V63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67"/>
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1432,7 +1433,7 @@
         <v>47</v>
       </c>
       <c r="G56">
-        <f t="shared" ref="G56:G64" si="5">B56-B55</f>
+        <f t="shared" ref="G56:G63" si="5">B56-B55</f>
         <v>16</v>
       </c>
       <c r="H56">
@@ -1591,18 +1592,28 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A63" s="1">
+      <c r="A63" s="4">
         <v>43970</v>
       </c>
       <c r="B63">
         <v>316</v>
       </c>
+      <c r="C63">
+        <v>789</v>
+      </c>
       <c r="D63" s="3">
         <v>16</v>
+      </c>
+      <c r="E63" s="3">
+        <v>91</v>
       </c>
       <c r="G63">
         <f t="shared" si="5"/>
         <v>16</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="6"/>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualização - 23 de maio
</commit_message>
<xml_diff>
--- a/corona.xlsx
+++ b/corona.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-Gamer\Desktop\corona\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7017581C-F455-40C2-8F47-FB5ED98B4714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEC6CE4-DC42-4745-973E-2018F1A0A7FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2140" yWindow="1090" windowWidth="38620" windowHeight="21000" xr2:uid="{4C98B353-EDBB-48FF-AC02-0102F8101F02}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{4C98B353-EDBB-48FF-AC02-0102F8101F02}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -412,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9475EA1A-E4F1-4D00-85AC-F11623C5E008}">
-  <dimension ref="A1:V63"/>
+  <dimension ref="A1:V67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1433,11 +1433,11 @@
         <v>47</v>
       </c>
       <c r="G56">
-        <f t="shared" ref="G56:G63" si="5">B56-B55</f>
+        <f t="shared" ref="G56:G67" si="5">B56-B55</f>
         <v>16</v>
       </c>
       <c r="H56">
-        <f t="shared" ref="H56:H63" si="6">C56-C55</f>
+        <f t="shared" ref="H56:H66" si="6">C56-C55</f>
         <v>47</v>
       </c>
     </row>
@@ -1614,6 +1614,96 @@
       <c r="H63">
         <f t="shared" si="6"/>
         <v>91</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" s="4">
+        <v>43971</v>
+      </c>
+      <c r="B64">
+        <v>330</v>
+      </c>
+      <c r="C64">
+        <v>834</v>
+      </c>
+      <c r="D64" s="3">
+        <v>14</v>
+      </c>
+      <c r="E64" s="3">
+        <v>45</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" s="4">
+        <v>43972</v>
+      </c>
+      <c r="B65">
+        <v>355</v>
+      </c>
+      <c r="C65">
+        <v>967</v>
+      </c>
+      <c r="D65" s="3">
+        <v>25</v>
+      </c>
+      <c r="E65" s="3">
+        <v>133</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="6"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" s="4">
+        <v>43973</v>
+      </c>
+      <c r="B66">
+        <v>373</v>
+      </c>
+      <c r="C66">
+        <v>1083</v>
+      </c>
+      <c r="D66" s="3">
+        <v>18</v>
+      </c>
+      <c r="E66" s="3">
+        <v>116</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="6"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67" s="4">
+        <v>43974</v>
+      </c>
+      <c r="B67">
+        <v>390</v>
+      </c>
+      <c r="D67" s="3">
+        <v>17</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="5"/>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>